<commit_message>
I18N Extenions for Table parser
</commit_message>
<xml_diff>
--- a/KSFramework/Product/SettingSource/StringsTable.xlsx
+++ b/KSFramework/Product/SettingSource/StringsTable.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace\KSFramework\KSFramework\Product\SettingSource\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13065"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28695" windowHeight="13065"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +30,7 @@
     <author>mrkelly</author>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0">
+    <comment ref="A3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -34,7 +39,7 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">mrkelly:
+          <t>mrkelly:
 主键可以是数字，也可以任何字符串。这里示例一个由两个列组合的主键</t>
         </r>
       </text>
@@ -44,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Id</t>
   </si>
@@ -82,14 +87,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="22">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="宋体"/>
@@ -108,132 +107,18 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="9"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="60"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="52"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color indexed="63"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="62"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="17"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color indexed="12"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color indexed="20"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
+      <sz val="9"/>
+      <color indexed="81"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color indexed="62"/>
+      <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color indexed="62"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="10"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color indexed="62"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color indexed="23"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color indexed="62"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color indexed="9"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color indexed="52"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-    </font>
   </fonts>
-  <fills count="18">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -246,98 +131,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="44"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="29"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="22"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="51"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="49"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="47"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="55"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="42"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="26"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="57"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="27"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="43"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="53"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="31"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="12">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -382,251 +177,9 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color indexed="52"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="63"/>
-      </left>
-      <right style="thin">
-        <color indexed="63"/>
-      </right>
-      <top style="thin">
-        <color indexed="63"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="63"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="23"/>
-      </left>
-      <right style="thin">
-        <color indexed="23"/>
-      </right>
-      <top style="thin">
-        <color indexed="23"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="23"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="22"/>
-      </left>
-      <right style="thin">
-        <color indexed="22"/>
-      </right>
-      <top style="thin">
-        <color indexed="22"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="22"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="49"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="44"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color indexed="63"/>
-      </left>
-      <right style="double">
-        <color indexed="63"/>
-      </right>
-      <top style="double">
-        <color indexed="63"/>
-      </top>
-      <bottom style="double">
-        <color indexed="63"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="49"/>
-      </top>
-      <bottom style="double">
-        <color indexed="49"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -659,57 +212,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -778,11 +285,19 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
@@ -796,7 +311,7 @@
       <xdr:row>32</xdr:row>
       <xdr:rowOff>57785</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="文本框 1"/>
         <xdr:cNvSpPr txBox="1"/>
@@ -838,13 +353,13 @@
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
           <a:noAutofit/>
         </a:bodyPr>
+        <a:lstStyle/>
         <a:p>
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
             <a:t>这里集合字符串，不做翻译；</a:t>
           </a:r>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
@@ -1176,6 +691,7 @@
           </a:gdLst>
           <a:ahLst/>
           <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
           <a:pathLst>
             <a:path w="21600" h="21600"/>
           </a:pathLst>
@@ -1208,26 +724,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="28.875" customWidth="1"/>
     <col min="2" max="2" width="29.375" customWidth="1"/>
     <col min="3" max="3" width="28.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1238,14 +752,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="6"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1256,7 +770,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
         <v>7</v>
       </c>
@@ -1265,56 +779,53 @@
       </c>
       <c r="C4" s="7"/>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A3:C6"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.510416666666667" footer="0.510416666666667"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51041666666666696" footer="0.51041666666666696"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter alignWithMargins="0" scaleWithDoc="0"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <headerFooter scaleWithDoc="0" alignWithMargins="0"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.510416666666667" footer="0.510416666666667"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51041666666666696" footer="0.51041666666666696"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter alignWithMargins="0" scaleWithDoc="0"/>
+  <headerFooter scaleWithDoc="0" alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.510416666666667" footer="0.510416666666667"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51041666666666696" footer="0.51041666666666696"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter alignWithMargins="0" scaleWithDoc="0"/>
+  <headerFooter scaleWithDoc="0" alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>